<commit_message>
updating excel loot values
</commit_message>
<xml_diff>
--- a/ADD Economy.xlsx
+++ b/ADD Economy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eddie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CS4043\CS4043 Game Design\At-Debts-Door-Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602B2827-CA8B-4D80-8188-AB8364E91676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C160C0-936B-4208-9721-49F6206034B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="12840" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{A19BE72B-50F3-4AFF-A937-1D682708FFF5}"/>
+    <workbookView xWindow="12870" yWindow="4545" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{A19BE72B-50F3-4AFF-A937-1D682708FFF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Levels" sheetId="1" r:id="rId1"/>
@@ -183,10 +183,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,7 +710,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -735,50 +736,80 @@
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B2" s="3">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B3" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B4" s="3">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B5" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="B6" s="3">
+        <v>250</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="B7" s="3">
+        <v>250</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="B8" s="3">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="B9" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="B10" s="3">
+        <v>200</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="B11" s="3">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>